<commit_message>
Workbook 1.1.6: Fix for missing ALN extension trailing zeroes (#4697)
* Fix for leading zeroes in merge script

* Bumping workbook versions to 1.1.6

* Updating cypress wb fixtures

* Removing dated cfda-lookup CSVs

* Reverting check_aln_prefix_pattern.py

* Lint
</commit_message>
<xml_diff>
--- a/backend/cypress/fixtures/test_workbooks/additional-ueis-workbook.xlsx
+++ b/backend/cypress/fixtures/test_workbooks/additional-ueis-workbook.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1.5</t>
+    <t xml:space="preserve">1.1.6</t>
   </si>
   <si>
     <t xml:space="preserve">Section</t>
@@ -449,7 +449,7 @@
   <dimension ref="A1:A1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="XFD12" activeCellId="0" sqref="XFD12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>